<commit_message>
creating test functions for kp problem
</commit_message>
<xml_diff>
--- a/test/mokp/instances/2kp250.xlsx
+++ b/test/mokp/instances/2kp250.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37609ee190385eca/Documentos/JosaFerreira/myJobs/02-projects/Jumento.jl/test/mokp/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7455AF-EC75-4BA9-AF8E-708EF44D5868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7455AF-EC75-4BA9-AF8E-708EF44D5868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3210" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" activeTab="4" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -7679,7 +7679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7695,7 +7695,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -12629,8 +12629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46539067-EAF6-46F5-A535-790CD20A21BA}">
   <dimension ref="A1:CSM2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:CSM2"/>
+    <sheetView tabSelected="1" topLeftCell="CSC1" workbookViewId="0">
+      <selection activeCell="CSM2" sqref="CSM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27855,7 +27855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F681E866-395D-4754-8FDD-4C98C228748A}">
   <dimension ref="A1:C569"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A565" workbookViewId="0">
+    <sheetView topLeftCell="A565" workbookViewId="0">
       <selection activeCell="A574" sqref="A570:A574"/>
     </sheetView>
   </sheetViews>

</xml_diff>